<commit_message>
modify time allocation.xlsx format
</commit_message>
<xml_diff>
--- a/documentation/Time allocation.xlsx
+++ b/documentation/Time allocation.xlsx
@@ -149,7 +149,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="[$NT$-404]#,##0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -169,6 +169,11 @@
     <font>
       <sz val="18"/>
       <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="11"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -246,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -471,6 +476,19 @@
       <left style="thin">
         <color indexed="17"/>
       </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -485,6 +503,17 @@
       <bottom style="thin">
         <color indexed="19"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -585,6 +614,19 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="19"/>
       </left>
       <right style="thin">
@@ -626,7 +668,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -636,10 +678,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -651,10 +693,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -663,13 +705,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -699,34 +741,25 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -735,67 +768,85 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -870,10 +921,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.448898"/>
+          <c:x val="0.439123"/>
           <c:y val="0"/>
-          <c:w val="0.102204"/>
-          <c:h val="0.111708"/>
+          <c:w val="0.121753"/>
+          <c:h val="0.108491"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -889,10 +940,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0305874"/>
-          <c:y val="0.111708"/>
-          <c:w val="0.964413"/>
-          <c:h val="0.786649"/>
+          <c:x val="0.0364379"/>
+          <c:y val="0.108491"/>
+          <c:w val="0.958562"/>
+          <c:h val="0.799351"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1262,7 +1313,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" i="0" strike="noStrike" sz="1000" u="none">
+              <a:defRPr b="0" i="0" strike="noStrike" sz="800" u="none">
                 <a:solidFill>
                   <a:srgbClr val="444444"/>
                 </a:solidFill>
@@ -1385,10 +1436,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14983"/>
-          <c:y val="0"/>
-          <c:w val="0.101656"/>
-          <c:h val="0.151336"/>
+          <c:x val="0.181962"/>
+          <c:y val="0.00274897"/>
+          <c:w val="0.118982"/>
+          <c:h val="0.164542"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1404,10 +1455,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.005"/>
-          <c:y val="0.151336"/>
-          <c:w val="0.401317"/>
-          <c:h val="0.836164"/>
+          <c:x val="0.053103"/>
+          <c:y val="0.167291"/>
+          <c:w val="0.376701"/>
+          <c:h val="0.717326"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1536,7 +1587,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="inEnd"/>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1568,7 +1619,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="inEnd"/>
+              <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1600,7 +1651,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="inEnd"/>
+              <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1632,7 +1683,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="inEnd"/>
+              <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1694,7 +1745,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1702,6 +1753,19 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="6350" cap="flat">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="400000"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1767,10 +1831,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.445465"/>
-          <c:y val="0.0672033"/>
-          <c:w val="0.554535"/>
-          <c:h val="0.270333"/>
+          <c:x val="0.470454"/>
+          <c:y val="0"/>
+          <c:w val="0.529546"/>
+          <c:h val="0.288075"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1845,10 +1909,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.361186"/>
+          <c:x val="0.336332"/>
           <c:y val="0"/>
-          <c:w val="0.277627"/>
-          <c:h val="0.0867606"/>
+          <c:w val="0.327337"/>
+          <c:h val="0.088971"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1864,10 +1928,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0859929"/>
-          <c:y val="0.0867606"/>
-          <c:w val="0.909007"/>
-          <c:h val="0.847953"/>
+          <c:x val="0.10139"/>
+          <c:y val="0.088971"/>
+          <c:w val="0.89361"/>
+          <c:h val="0.844398"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2427,10 +2491,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.327625"/>
+          <c:x val="0.325889"/>
           <c:y val="0"/>
-          <c:w val="0.34475"/>
-          <c:h val="0.135467"/>
+          <c:w val="0.348223"/>
+          <c:h val="0.138918"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2446,10 +2510,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.128177"/>
-          <c:y val="0.135467"/>
-          <c:w val="0.866823"/>
-          <c:h val="0.769613"/>
+          <c:x val="0.129468"/>
+          <c:y val="0.138918"/>
+          <c:w val="0.865532"/>
+          <c:h val="0.764062"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2891,10 +2955,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.283406"/>
+          <c:x val="0.202015"/>
           <c:y val="0"/>
-          <c:w val="0.39455"/>
-          <c:h val="0.119769"/>
+          <c:w val="0.508128"/>
+          <c:h val="0.116539"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2910,10 +2974,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.122599"/>
-          <c:y val="0.119769"/>
-          <c:w val="0.838692"/>
-          <c:h val="0.677395"/>
+          <c:x val="0.185277"/>
+          <c:y val="0.116539"/>
+          <c:w val="0.699405"/>
+          <c:h val="0.633968"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3314,9 +3378,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0"/>
-          <c:y val="0.934273"/>
+          <c:y val="0.883918"/>
           <c:w val="1"/>
-          <c:h val="0.0657266"/>
+          <c:h val="0.116082"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3391,10 +3455,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.368491"/>
+          <c:x val="0.346075"/>
           <c:y val="0"/>
-          <c:w val="0.263019"/>
-          <c:h val="0.135467"/>
+          <c:w val="0.30785"/>
+          <c:h val="0.138918"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3410,10 +3474,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.126781"/>
-          <c:y val="0.135467"/>
-          <c:w val="0.821536"/>
-          <c:h val="0.769613"/>
+          <c:x val="0.147851"/>
+          <c:y val="0.138918"/>
+          <c:w val="0.791878"/>
+          <c:h val="0.764062"/>
         </c:manualLayout>
       </c:layout>
       <c:areaChart>
@@ -3846,10 +3910,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.451587"/>
+          <c:x val="0.445092"/>
           <c:y val="0"/>
-          <c:w val="0.0968269"/>
-          <c:h val="0.124804"/>
+          <c:w val="0.109815"/>
+          <c:h val="0.127984"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3865,10 +3929,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0688831"/>
-          <c:y val="0.124804"/>
-          <c:w val="0.87399"/>
-          <c:h val="0.70215"/>
+          <c:x val="0.0781232"/>
+          <c:y val="0.127984"/>
+          <c:w val="0.857087"/>
+          <c:h val="0.694881"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3980,7 +4044,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="6"/>
+            <c:size val="72"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4276,10 +4340,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.262599"/>
-          <c:y val="0.932035"/>
-          <c:w val="0.516333"/>
-          <c:h val="0.0679645"/>
+          <c:x val="0.252105"/>
+          <c:y val="0.930622"/>
+          <c:w val="0.538323"/>
+          <c:h val="0.0693776"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4354,10 +4418,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.448762"/>
+          <c:x val="0.441722"/>
           <c:y val="0"/>
-          <c:w val="0.102476"/>
-          <c:h val="0.116784"/>
+          <c:w val="0.116556"/>
+          <c:h val="0.119759"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4373,10 +4437,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0562806"/>
-          <c:y val="0.116784"/>
-          <c:w val="0.935303"/>
-          <c:h val="0.721813"/>
+          <c:x val="0.0640135"/>
+          <c:y val="0.119759"/>
+          <c:w val="0.926414"/>
+          <c:h val="0.715044"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4744,10 +4808,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.449101"/>
+          <c:x val="0.441671"/>
           <c:y val="0"/>
-          <c:w val="0.101798"/>
-          <c:h val="0.152196"/>
+          <c:w val="0.116658"/>
+          <c:h val="0.15316"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4763,10 +4827,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0639637"/>
-          <c:y val="0.152196"/>
-          <c:w val="0.899773"/>
-          <c:h val="0.709809"/>
+          <c:x val="0.0733007"/>
+          <c:y val="0.15316"/>
+          <c:w val="0.886571"/>
+          <c:h val="0.705206"/>
         </c:manualLayout>
       </c:layout>
       <c:bubbleChart>
@@ -5118,15 +5182,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1084</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>21614</xdr:rowOff>
+      <xdr:rowOff>46303</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>358521</xdr:colOff>
+      <xdr:colOff>364492</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>218842</xdr:rowOff>
+      <xdr:rowOff>104872</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5134,8 +5198,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1084" y="2824504"/>
-        <a:ext cx="9526838" cy="2998213"/>
+        <a:off x="-1" y="2849193"/>
+        <a:ext cx="7997194" cy="2859553"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5148,15 +5212,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>987060</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>174124</xdr:rowOff>
+      <xdr:colOff>740083</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>353504</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>152012</xdr:rowOff>
+      <xdr:rowOff>151299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5164,8 +5228,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="987060" y="6541902"/>
-        <a:ext cx="6414945" cy="3033507"/>
+        <a:off x="740083" y="6745763"/>
+        <a:ext cx="5480822" cy="2828933"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5180,13 +5244,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>151909</xdr:rowOff>
+      <xdr:rowOff>44069</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4559300</xdr:colOff>
+      <xdr:colOff>3893026</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>85859</xdr:rowOff>
+      <xdr:rowOff>211699</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5195,8 +5259,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19050" y="1025034"/>
-          <a:ext cx="4559300" cy="593081"/>
+          <a:off x="-19050" y="917194"/>
+          <a:ext cx="3893026" cy="826761"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5359,13 +5423,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>13707</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>419608</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>2008867</xdr:rowOff>
+      <xdr:colOff>495808</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101589</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5374,8 +5438,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19051" y="13707"/>
-          <a:ext cx="4648710" cy="1995161"/>
+          <a:off x="-19051" y="-175840"/>
+          <a:ext cx="4051810" cy="2696201"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5664,15 +5728,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>800781</xdr:colOff>
+      <xdr:colOff>743990</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>386752</xdr:rowOff>
+      <xdr:rowOff>386751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>895782</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19239</xdr:rowOff>
+      <xdr:colOff>860091</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>176698</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5680,8 +5744,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5029881" y="386752"/>
-        <a:ext cx="4209802" cy="3860318"/>
+        <a:off x="4299990" y="386751"/>
+        <a:ext cx="3570502" cy="3764413"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5700,14 +5764,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>131206</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>356741</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4648200</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>175646</xdr:rowOff>
+      <xdr:rowOff>37326</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5716,8 +5780,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19050" y="495061"/>
-          <a:ext cx="4648200" cy="1060441"/>
+          <a:off x="-19050" y="356741"/>
+          <a:ext cx="4724400" cy="1060441"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5873,15 +5937,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>6285</xdr:colOff>
+      <xdr:colOff>6283</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>28727</xdr:rowOff>
+      <xdr:rowOff>28726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2830607</xdr:colOff>
+      <xdr:colOff>2802434</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>209371</xdr:rowOff>
+      <xdr:rowOff>147947</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5889,8 +5953,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6285" y="3191027"/>
-        <a:ext cx="2824323" cy="2472359"/>
+        <a:off x="6283" y="3191026"/>
+        <a:ext cx="2796152" cy="2410936"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5903,15 +5967,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3244787</xdr:colOff>
+      <xdr:colOff>3054286</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>28680</xdr:rowOff>
+      <xdr:rowOff>28681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1708</xdr:colOff>
+      <xdr:colOff>192207</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>24117</xdr:rowOff>
+      <xdr:rowOff>101626</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5919,8 +5983,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3244786" y="3190981"/>
-        <a:ext cx="2954523" cy="2796421"/>
+        <a:off x="3054286" y="3190981"/>
+        <a:ext cx="2294122" cy="2873930"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5933,15 +5997,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>237991</xdr:colOff>
+      <xdr:colOff>175195</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>28727</xdr:rowOff>
+      <xdr:rowOff>28726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>121602</xdr:colOff>
+      <xdr:colOff>147198</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>209371</xdr:rowOff>
+      <xdr:rowOff>147947</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5949,8 +6013,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6435591" y="3191027"/>
-        <a:ext cx="2855412" cy="2472359"/>
+        <a:off x="5331395" y="3191026"/>
+        <a:ext cx="2448504" cy="2410936"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5970,13 +6034,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>342661</xdr:rowOff>
+      <xdr:rowOff>51941</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4648200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>178186</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>140831</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5985,8 +6049,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19050" y="342661"/>
-          <a:ext cx="4648200" cy="2228841"/>
+          <a:off x="-19050" y="51941"/>
+          <a:ext cx="4724400" cy="2228841"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6182,15 +6246,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9079</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>229448</xdr:rowOff>
+      <xdr:rowOff>229446</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1677730</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>412576</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>112055</xdr:rowOff>
+      <xdr:rowOff>45381</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6198,8 +6262,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9079" y="4398858"/>
-        <a:ext cx="9009252" cy="2683591"/>
+        <a:off x="-1" y="4398856"/>
+        <a:ext cx="7943677" cy="2616919"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6218,14 +6282,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>55006</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>219581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4648200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>60076</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114161</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6234,8 +6298,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19050" y="418861"/>
-          <a:ext cx="4648200" cy="1527801"/>
+          <a:off x="-19050" y="219581"/>
+          <a:ext cx="4724400" cy="1527801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6431,15 +6495,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1055</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>80265</xdr:rowOff>
+      <xdr:rowOff>80263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2097221</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>407275</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>147170</xdr:rowOff>
+      <xdr:rowOff>75920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6447,8 +6511,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1055" y="3997579"/>
-        <a:ext cx="9144667" cy="2867890"/>
+        <a:off x="-1" y="3997577"/>
+        <a:ext cx="8039977" cy="2796641"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6467,14 +6531,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>39766</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>173861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4699000</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>25151</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>48756</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6483,8 +6547,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19050" y="403621"/>
-          <a:ext cx="4699000" cy="1761481"/>
+          <a:off x="-19050" y="173861"/>
+          <a:ext cx="4775200" cy="1761481"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6682,13 +6746,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>216546</xdr:rowOff>
+      <xdr:rowOff>227947</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1403177</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>54461</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>339234</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>224630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6696,8 +6760,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="-1" y="3625861"/>
-        <a:ext cx="9150179" cy="3402804"/>
+        <a:off x="-1" y="3637262"/>
+        <a:ext cx="7984636" cy="3306937"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6941,10 +7005,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue"/>
-            <a:ea typeface="Helvetica Neue"/>
-            <a:cs typeface="Helvetica Neue"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -7512,10 +7576,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue"/>
-            <a:ea typeface="Helvetica Neue"/>
-            <a:cs typeface="Helvetica Neue"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -7773,14 +7837,14 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.8333" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.8" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="64.6719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.8516" style="1" customWidth="1"/>
-    <col min="6" max="256" width="27.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="64.6016" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.8125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.8125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.8125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.8125" style="1" customWidth="1"/>
+    <col min="6" max="256" width="27.8125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.65" customHeight="1">
@@ -8086,23 +8150,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.6" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="23" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="23" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="23" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="23" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="23" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="23" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="23" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="23" customWidth="1"/>
-    <col min="10" max="10" width="13.5" style="23" customWidth="1"/>
-    <col min="11" max="256" width="13.5" style="23" customWidth="1"/>
+    <col min="1" max="1" width="13.6016" style="23" customWidth="1"/>
+    <col min="2" max="2" width="10.6016" style="23" customWidth="1"/>
+    <col min="3" max="3" width="10.6016" style="23" customWidth="1"/>
+    <col min="4" max="4" width="10.6016" style="23" customWidth="1"/>
+    <col min="5" max="5" width="10.6016" style="23" customWidth="1"/>
+    <col min="6" max="6" width="13.6016" style="23" customWidth="1"/>
+    <col min="7" max="7" width="13.6016" style="23" customWidth="1"/>
+    <col min="8" max="8" width="13.6016" style="23" customWidth="1"/>
+    <col min="9" max="9" width="13.6016" style="23" customWidth="1"/>
+    <col min="10" max="10" width="13.6016" style="23" customWidth="1"/>
+    <col min="11" max="11" width="13.6016" style="23" customWidth="1"/>
+    <col min="12" max="256" width="13.6016" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="204.3" customHeight="1">
@@ -8116,35 +8181,37 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="6"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" ht="28.65" customHeight="1">
-      <c r="A2" t="s" s="24">
+      <c r="A2" t="s" s="25">
         <v>9</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="11"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" t="s" s="8">
         <v>10</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="28">
         <v>2012</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="28">
         <v>2013</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="28">
         <v>2014</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="29">
         <v>2015</v>
       </c>
       <c r="F3" s="10"/>
@@ -8152,21 +8219,22 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="11"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="30">
         <v>25</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="31">
         <v>50</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="31">
         <v>100</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="32">
         <v>75</v>
       </c>
       <c r="F4" s="10"/>
@@ -8174,21 +8242,22 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="11"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" ht="19.95" customHeight="1">
       <c r="A5" t="s" s="14">
         <v>12</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="33">
         <v>50</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="34">
         <v>100</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="34">
         <v>150</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="35">
         <v>100</v>
       </c>
       <c r="F5" s="10"/>
@@ -8196,21 +8265,22 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="11"/>
+      <c r="K5" s="27"/>
     </row>
     <row r="6" ht="19.95" customHeight="1">
       <c r="A6" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="36">
         <v>100</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="37">
         <v>200</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="37">
         <v>250</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="38">
         <v>350</v>
       </c>
       <c r="F6" s="10"/>
@@ -8218,21 +8288,22 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="11"/>
+      <c r="K6" s="27"/>
     </row>
     <row r="7" ht="19.95" customHeight="1">
       <c r="A7" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="33">
         <v>75</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="34">
         <v>100</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="34">
         <v>150</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="35">
         <v>200</v>
       </c>
       <c r="F7" s="10"/>
@@ -8240,9 +8311,10 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="11"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="37"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -8252,6 +8324,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="11"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="17"/>
@@ -8264,6 +8337,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="11"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="20"/>
@@ -8276,6 +8350,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="22"/>
+      <c r="K10" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8299,15 +8374,15 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.6667" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.6" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="64.6719" style="38" customWidth="1"/>
-    <col min="2" max="2" width="16.6719" style="38" customWidth="1"/>
-    <col min="3" max="3" width="13" style="38" customWidth="1"/>
-    <col min="4" max="4" width="13" style="38" customWidth="1"/>
-    <col min="5" max="5" width="13" style="38" customWidth="1"/>
-    <col min="6" max="6" width="16.6719" style="38" customWidth="1"/>
-    <col min="7" max="256" width="16.6719" style="38" customWidth="1"/>
+    <col min="1" max="1" width="64.6016" style="41" customWidth="1"/>
+    <col min="2" max="2" width="16.6016" style="41" customWidth="1"/>
+    <col min="3" max="3" width="13" style="41" customWidth="1"/>
+    <col min="4" max="4" width="13" style="41" customWidth="1"/>
+    <col min="5" max="5" width="13" style="41" customWidth="1"/>
+    <col min="6" max="6" width="16.6016" style="41" customWidth="1"/>
+    <col min="7" max="256" width="16.6016" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.65" customHeight="1">
@@ -8325,64 +8400,64 @@
       <c r="B2" t="s" s="8">
         <v>10</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="28">
         <v>2012</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="28">
         <v>2013</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="29">
         <v>2014</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" t="s" s="12">
         <v>16</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="30">
         <v>25</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="31">
         <v>50</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="32">
         <v>25</v>
       </c>
-      <c r="F3" s="39"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" ht="19.95" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" t="s" s="14">
         <v>17</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="33">
         <v>50</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="34">
         <v>100</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="35">
         <v>150</v>
       </c>
-      <c r="F4" s="39"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" ht="19.95" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" t="s" s="14">
         <v>18</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="36">
         <v>100</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="37">
         <v>200</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="38">
         <v>250</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="17"/>
@@ -8558,14 +8633,14 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.6" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="64.6719" style="40" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="40" customWidth="1"/>
-    <col min="3" max="3" width="22.1719" style="40" customWidth="1"/>
-    <col min="4" max="4" width="22.1719" style="40" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="40" customWidth="1"/>
-    <col min="6" max="256" width="9.5" style="40" customWidth="1"/>
+    <col min="1" max="1" width="64.6016" style="43" customWidth="1"/>
+    <col min="2" max="2" width="9.60156" style="43" customWidth="1"/>
+    <col min="3" max="3" width="22.2109" style="43" customWidth="1"/>
+    <col min="4" max="4" width="22.2109" style="43" customWidth="1"/>
+    <col min="5" max="5" width="9.60156" style="43" customWidth="1"/>
+    <col min="6" max="256" width="9.60156" style="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.65" customHeight="1">
@@ -8580,169 +8655,169 @@
     <row r="2" ht="20.05" customHeight="1">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" t="s" s="41">
+      <c r="C2" t="s" s="44">
         <v>20</v>
       </c>
       <c r="D2" t="s" s="9">
         <v>21</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" t="s" s="12">
         <v>22</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="45">
         <v>3.01</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="32">
         <v>58</v>
       </c>
-      <c r="E3" s="39"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" ht="19.95" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" t="s" s="14">
         <v>23</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="46">
         <v>3.22</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="35">
         <v>62</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" ht="19.95" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" t="s" s="14">
         <v>24</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="47">
         <v>2.54</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="38">
         <v>66</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" ht="19.95" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" t="s" s="14">
         <v>25</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="46">
         <v>1.18</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="35">
         <v>69</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" ht="19.95" customHeight="1">
       <c r="A7" s="7"/>
       <c r="B7" t="s" s="14">
         <v>26</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="47">
         <v>0.51</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="38">
         <v>74</v>
       </c>
-      <c r="E7" s="39"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" ht="19.95" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" t="s" s="14">
         <v>27</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="46">
         <v>0.1</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="35">
         <v>79</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" ht="19.95" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" t="s" s="14">
         <v>28</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="47">
         <v>0.02</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="38">
         <v>82</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" ht="19.95" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" t="s" s="14">
         <v>29</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="46">
         <v>0.02</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="35">
         <v>82</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" ht="19.95" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" t="s" s="14">
         <v>30</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="47">
         <v>0.18</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="38">
         <v>80</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" ht="19.95" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" t="s" s="14">
         <v>31</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="46">
         <v>0.8</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="35">
         <v>74</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="42"/>
     </row>
     <row r="13" ht="19.95" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" t="s" s="14">
         <v>32</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="47">
         <v>1.68</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="38">
         <v>64</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="42"/>
     </row>
     <row r="14" ht="19.95" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" t="s" s="14">
         <v>33</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="46">
         <v>2.61</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="35">
         <v>58</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="42"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" s="17"/>
@@ -8864,14 +8939,14 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.8333" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.8" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="64.6719" style="45" customWidth="1"/>
-    <col min="2" max="2" width="27.8516" style="45" customWidth="1"/>
-    <col min="3" max="3" width="27.8516" style="45" customWidth="1"/>
-    <col min="4" max="4" width="27.8516" style="45" customWidth="1"/>
-    <col min="5" max="5" width="27.8516" style="45" customWidth="1"/>
-    <col min="6" max="256" width="27.8516" style="45" customWidth="1"/>
+    <col min="1" max="1" width="64.6016" style="48" customWidth="1"/>
+    <col min="2" max="2" width="27.8125" style="48" customWidth="1"/>
+    <col min="3" max="3" width="27.8125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="27.8125" style="48" customWidth="1"/>
+    <col min="5" max="5" width="27.8125" style="48" customWidth="1"/>
+    <col min="6" max="256" width="27.8125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.65" customHeight="1">
@@ -8885,7 +8960,7 @@
     </row>
     <row r="2" ht="20.05" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" t="s" s="46">
+      <c r="B2" t="s" s="49">
         <v>36</v>
       </c>
       <c r="C2" t="s" s="9">
@@ -8896,10 +8971,10 @@
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" s="7"/>
-      <c r="B3" s="47">
+      <c r="B3" s="50">
         <v>25</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="32">
         <v>13</v>
       </c>
       <c r="D3" s="10"/>
@@ -8907,10 +8982,10 @@
     </row>
     <row r="4" ht="19.95" customHeight="1">
       <c r="A4" s="7"/>
-      <c r="B4" s="48">
+      <c r="B4" s="51">
         <v>28</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="35">
         <v>12</v>
       </c>
       <c r="D4" s="10"/>
@@ -8918,10 +8993,10 @@
     </row>
     <row r="5" ht="19.95" customHeight="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="49">
+      <c r="B5" s="52">
         <v>34</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="38">
         <v>17</v>
       </c>
       <c r="D5" s="10"/>
@@ -8929,10 +9004,10 @@
     </row>
     <row r="6" ht="19.95" customHeight="1">
       <c r="A6" s="7"/>
-      <c r="B6" s="48">
+      <c r="B6" s="51">
         <v>35</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="35">
         <v>18</v>
       </c>
       <c r="D6" s="10"/>
@@ -8940,10 +9015,10 @@
     </row>
     <row r="7" ht="19.95" customHeight="1">
       <c r="A7" s="7"/>
-      <c r="B7" s="49">
+      <c r="B7" s="52">
         <v>43</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="38">
         <v>18</v>
       </c>
       <c r="D7" s="10"/>
@@ -8951,10 +9026,10 @@
     </row>
     <row r="8" ht="19.95" customHeight="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="48">
+      <c r="B8" s="51">
         <v>48</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="35">
         <v>21</v>
       </c>
       <c r="D8" s="10"/>
@@ -8962,10 +9037,10 @@
     </row>
     <row r="9" ht="19.95" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="49">
+      <c r="B9" s="52">
         <v>55</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="38">
         <v>26</v>
       </c>
       <c r="D9" s="10"/>
@@ -8973,10 +9048,10 @@
     </row>
     <row r="10" ht="19.95" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="48">
+      <c r="B10" s="51">
         <v>62</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="35">
         <v>30</v>
       </c>
       <c r="D10" s="10"/>
@@ -8984,10 +9059,10 @@
     </row>
     <row r="11" ht="19.95" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="49">
+      <c r="B11" s="52">
         <v>65</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="38">
         <v>29</v>
       </c>
       <c r="D11" s="10"/>
@@ -8995,10 +9070,10 @@
     </row>
     <row r="12" ht="19.95" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="48">
+      <c r="B12" s="51">
         <v>67</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="35">
         <v>28</v>
       </c>
       <c r="D12" s="10"/>
@@ -9131,14 +9206,14 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.5" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.6" defaultRowHeight="20.05" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="64.6719" style="50" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="50" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="50" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="50" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="50" customWidth="1"/>
-    <col min="6" max="256" width="18.5" style="50" customWidth="1"/>
+    <col min="1" max="1" width="64.6016" style="53" customWidth="1"/>
+    <col min="2" max="2" width="18.6016" style="53" customWidth="1"/>
+    <col min="3" max="3" width="18.6016" style="53" customWidth="1"/>
+    <col min="4" max="4" width="18.6016" style="53" customWidth="1"/>
+    <col min="5" max="5" width="18.6016" style="53" customWidth="1"/>
+    <col min="6" max="256" width="18.6016" style="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.65" customHeight="1">
@@ -9152,133 +9227,133 @@
     </row>
     <row r="2" ht="20.05" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" t="s" s="46">
+      <c r="B2" t="s" s="49">
         <v>39</v>
       </c>
-      <c r="C2" t="s" s="41">
+      <c r="C2" t="s" s="44">
         <v>40</v>
       </c>
       <c r="D2" t="s" s="9">
         <v>41</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
       <c r="A3" s="7"/>
-      <c r="B3" s="51">
+      <c r="B3" s="54">
         <v>8</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="31">
         <v>264</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="55">
         <v>7010784</v>
       </c>
-      <c r="E3" s="39"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" ht="19.95" customHeight="1">
       <c r="A4" s="7"/>
-      <c r="B4" s="53">
+      <c r="B4" s="56">
         <v>14</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="34">
         <v>378</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="57">
         <v>5352858</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" ht="19.95" customHeight="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="55">
+      <c r="B5" s="58">
         <v>11</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="37">
         <v>210</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="59">
         <v>5918000</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" ht="19.95" customHeight="1">
       <c r="A6" s="7"/>
-      <c r="B6" s="53">
+      <c r="B6" s="56">
         <v>10</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="34">
         <v>270</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="57">
         <v>6974910</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" ht="19.95" customHeight="1">
       <c r="A7" s="7"/>
-      <c r="B7" s="55">
+      <c r="B7" s="58">
         <v>4</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="37">
         <v>105</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="59">
         <v>2964150</v>
       </c>
-      <c r="E7" s="39"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" ht="19.95" customHeight="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="53">
+      <c r="B8" s="56">
         <v>13</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="34">
         <v>286</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="57">
         <v>3897894</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" ht="19.95" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="55">
+      <c r="B9" s="58">
         <v>5</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="37">
         <v>190</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="59">
         <v>4686350</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" ht="19.95" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="53">
+      <c r="B10" s="56">
         <v>7</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="34">
         <v>133</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="57">
         <v>1844843</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" ht="19.95" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="55">
+      <c r="B11" s="58">
         <v>12</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="37">
         <v>384</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="59">
         <v>11382528</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="42"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="17"/>

</xml_diff>